<commit_message>
Created BaseInputController Created Registration Created Localization Created Roles and Users
</commit_message>
<xml_diff>
--- a/RatingUniversity/Files/11_kolichestvo_izdannoy_uchebnoy_literaturi.xlsx
+++ b/RatingUniversity/Files/11_kolichestvo_izdannoy_uchebnoy_literaturi.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dilechka\Desktop\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="monografiya" sheetId="1" r:id="rId1"/>
@@ -32,7 +27,7 @@
     <definedName name="ucheb_name">monografiya!#REF!</definedName>
     <definedName name="ucheb_number">monografiya!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
   <si>
     <t>Ихтисослик шифри ва номи</t>
   </si>
@@ -84,9 +79,6 @@
   </si>
   <si>
     <t>М А Ъ Л У М О Т</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                  Жами</t>
   </si>
   <si>
     <t>Асосий штатдаги профессор-ўқитувчиларнинг 2014 йилда нашр этган монография,</t>
@@ -195,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -303,26 +295,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -352,11 +329,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -364,24 +359,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -393,12 +370,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -672,7 +643,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -680,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F17"/>
+  <dimension ref="A2:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -698,85 +669,85 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:6" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="15" t="s">
+      <c r="E8" s="18"/>
+      <c r="F8" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="16"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
@@ -828,51 +799,29 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="12">
-        <f>SUM(C11:C13)</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="12">
-        <f t="shared" ref="D14:F14" si="0">SUM(D11:D13)</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="25" t="s">
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="C16"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="26" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -883,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -899,85 +848,85 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:6" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="17" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="21"/>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="16"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
@@ -1029,41 +978,28 @@
       <c r="E13" s="3"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="12">
-        <f>SUM(C11:C13)</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="12">
-        <f t="shared" ref="D14:F14" si="0">SUM(D11:D13)</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1071,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F14"/>
+  <dimension ref="A2:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="B15" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1089,85 +1025,85 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:6" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="15" t="s">
+      <c r="E8" s="18"/>
+      <c r="F8" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="16"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
@@ -1219,40 +1155,28 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="12">
-        <f>SUM(C11:C13)</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="12">
-        <f>SUM(D11:D13)</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="12">
-        <f t="shared" ref="E14:F14" si="0">SUM(E11:E13)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1260,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F14"/>
+  <dimension ref="A2:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1278,85 +1202,85 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:6" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="24"/>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="16"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
@@ -1408,40 +1332,28 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="12">
-        <f>SUM(C11:C13)</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="12">
-        <f t="shared" ref="D14:F14" si="0">SUM(D11:D13)</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>